<commit_message>
Updated Sheet 23 Response
</commit_message>
<xml_diff>
--- a/Sheet.xlsx
+++ b/Sheet.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="215">
   <si>
     <t>Timestamp</t>
   </si>
@@ -554,6 +554,207 @@
   </si>
   <si>
     <t>Alles gut!</t>
+  </si>
+  <si>
+    <t>khuderanjit99@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I prefer project-based assessments because they align more closely with my learning style. They allow me to apply knowledge creatively, work at my own pace, and demonstrate understanding through practical outcomes rather than just memorizing content for a test. This method feels more meaningful and fair, especially for complex subjects.
+</t>
+  </si>
+  <si>
+    <t>One positive experience I had was during a group project in a science class. We designed an experiment and presented our findings. It worked well because it encouraged collaboration, critical thinking, and hands-on application of what we had learned. I felt more engaged and retained the information better than I would have through a written test.</t>
+  </si>
+  <si>
+    <t>One of the biggest challenges with traditional essays is the time pressure and the vague nature of some prompts. It can be frustrating trying to guess what the evaluator is really looking for. There's also a lot of pressure to write in a specific academic style that doesn’t always reflect how well I understand the topic.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I find oral assessments a bit stressful due to performance anxiety and fear of being put on the spot. However, when I’ve had time to prepare, they’ve also been helpful for developing confidence and improving my communication skills. The stress mostly comes from uncertainty about the questions or how the evaluator will react.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Project-based assessments do a better job of showing what I’ve actually learned, especially when it comes to practical skills and problem-solving. They also give room for creativity and teamwork, which aren’t captured well in tests or essays. It’s easier to show effort and depth of understanding in a project than in a time-limited exam.
+</t>
+  </si>
+  <si>
+    <t>Yes, I think traditional written assessments, especially take-home essays, can tempt students to use AI tools or plagiarize because it's easy to do and hard to detect. In contrast, project-based or oral assessments are more personalized and interactive, which makes dishonesty harder and less appealing. They tend to reflect genuine effort more clearly.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">My ideal assessment would combine a short written reflection, a creative project, and a brief oral presentation. This mix would allow me to explain my ideas clearly in writing, apply them in a practical way, and demonstrate understanding through spoken communication. It would reflect both what I know and how I think, offering a more complete picture of my learning.
+</t>
+  </si>
+  <si>
+    <t>emolebhai@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I prefer oral or presentation-based assessments because they allow me to explain my thinking in real time. I often understand a topic well but struggle to express it clearly in writing. Speaking gives me a chance to clarify my ideas, adapt to follow-up questions, and feel more involved in the evaluation process. It feels more personal and fair.
+</t>
+  </si>
+  <si>
+    <t>A positive experience I had was during a class debate. It was technically an oral assessment, but in a discussion format. It worked well because I had time to research, organize my arguments, and respond to opposing views. It made me think critically, and the interaction made learning more dynamic and memorable.</t>
+  </si>
+  <si>
+    <t>What frustrates me most is that essays often feel disconnected from how we use knowledge in real life. There’s pressure to use a specific format and vocabulary, and sometimes it feels more like a test of writing skills than understanding. Also, if the prompt is unclear, it’s hard to know if you're even answering it correctly.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I’ve found them both helpful and a bit stressful. The helpful part is that I can show how well I know the topic through my own words and examples. The stress usually comes from nervousness, especially in front of a class or when I’m unsure how much detail is expected. But overall, I think the interaction helps deepen understanding.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">They definitely show a broader range of what I’ve learned. With projects, I can demonstrate how I apply knowledge, not just recall it. I also enjoy being able to choose a topic or format that fits my interests or strengths. They often involve more time and effort, but the learning feels more real and lasting.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes, I think the format matters a lot. For example, generic essays can be tempting to outsource or generate with AI, especially if students feel lost. But assessments that involve personal input, creativity, or direct interaction (like presentations or unique projects) make dishonesty harder and less attractive. They feel more “customized,” so copying doesn’t really work.
+</t>
+  </si>
+  <si>
+    <t>My ideal format would blend a structured written part with an interactive component like a Q&amp;A or group discussion. I’d like clear criteria, chances to ask for feedback, and maybe even options to choose between formats. That way, students could play to their strengths while still showing real understanding and effort.</t>
+  </si>
+  <si>
+    <t>ronishadesai@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I prefer project-based assessments because they allow me to learn by doing, which matches my hands-on learning style. Projects give me the chance to apply what I’ve learned in a real-world or creative way, making the content more meaningful and easier to remember. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">One positive experience I had was with a project-based assessment in a science class. We had to design and present a model of an eco-friendly home, explaining how it worked and why we made certain choices. What made it work well for me was the freedom to be creative and the chance to work at my own pace. </t>
+  </si>
+  <si>
+    <t>What I find most challenging about traditional essay-based assessments is the time pressure and the struggle to clearly organize my thoughts quickly. Sometimes, even if I understand the topic well, I find it hard to express everything in a structured way under a strict time limit.</t>
+  </si>
+  <si>
+    <t>I’ve found oral assessments to be both helpful and stressful. They’re helpful because they push me to really understand the material—since I have to explain it clearly and answer questions on the spot. It also improves my communication skills and confidence over time.</t>
+  </si>
+  <si>
+    <t>Project-based or performance-based assessments often do a much better job of showing what I’ve truly learned compared to traditional tests or essays. They allow me to demonstrate practical skills, like problem-solving, critical thinking, and creativity, which aren’t always visible in written formats.</t>
+  </si>
+  <si>
+    <t>Yes, I think certain assessment formats can encourage or discourage academic dishonesty, especially with tools like AI becoming more accessible. For example, traditional written assignments or essays are more likely to tempt students to use AI tools to write for them—mainly because it’s easy to copy and paste, and sometimes the questions are so broad or repetitive that it doesn’t feel personal or meaningful.</t>
+  </si>
+  <si>
+    <t>My ideal assessment format would be a combination of a project, a short reflection, and a brief presentation.
+	•	The project would let me apply what I’ve learned in a creative or practical way—like building something, designing a solution, or exploring a topic deeply.</t>
+  </si>
+  <si>
+    <t>bhuvaasmita152@gmail.com</t>
+  </si>
+  <si>
+    <t>real time feedback</t>
+  </si>
+  <si>
+    <t>An oral assessment with real-time feedback gave me instant insights, boosted my confidence, and turned evaluation into a valuable learning exchange.</t>
+  </si>
+  <si>
+    <t>Time pressure, unclear questions, writing-skill bias, plagiarism risk, and limited real-world relevance.</t>
+  </si>
+  <si>
+    <t>Helpful due to real-time interaction and feedback, but stressful from confidence and language pressure.</t>
+  </si>
+  <si>
+    <t>Project-based assessments better showcase practical skills, creativity, sustained effort, and teamwork than traditional formats.</t>
+  </si>
+  <si>
+    <t>Yes — written assessments may tempt AI or plagiarism use due to ease and low detection, while oral and project-based formats discourage it through real-time interaction and observable work.</t>
+  </si>
+  <si>
+    <t>Project work plus oral exam for practical skills, understanding, and fairness.</t>
+  </si>
+  <si>
+    <t>kevalakbari2015@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Because easy to give answers and get result instantly </t>
+  </si>
+  <si>
+    <t>Oral</t>
+  </si>
+  <si>
+    <t>Sonetimes language</t>
+  </si>
+  <si>
+    <t>Effort</t>
+  </si>
+  <si>
+    <t>Yes, certain formats like take-home essays or online quizzes can encourage dishonesty due to easy access to AI tools and low risk of detection. In contrast, in-class exams or oral assessments discourage cheating by limiting resources and allowing real-time evaluation.</t>
+  </si>
+  <si>
+    <t>My ideal assessment would combine open-ended, real-world tasks with in-person presentations. This format promotes critical thinking, limits AI overuse, and allows instructors to assess understanding through dialogue, reducing cheating while encouraging authentic learning.</t>
+  </si>
+  <si>
+    <t>harshkukadiya2023@gmail.com</t>
+  </si>
+  <si>
+    <t>I’m not sure / New to these types</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Projects lead me to find a deep understanding and also real time experience </t>
+  </si>
+  <si>
+    <t>I've been doing projects all over my education and it's the best I'd say, essays are too old school.</t>
+  </si>
+  <si>
+    <t>We first of all, have to understand the topic, the deepness, what exactly the person want from us, which can be Little time consuming and, students being students, they'll seek for some already generated content to get a help and that leads to plagiarism.</t>
+  </si>
+  <si>
+    <t>It's helpful at some extent but totally stressful.</t>
+  </si>
+  <si>
+    <t>The knowledge we have, we have to apply it to the real time system, which leads to hands on experience and also help in future industry.</t>
+  </si>
+  <si>
+    <t>Yes, no doubt, a assessment fromat likr essay and all, Students do is all about getting content from one end to writing it on another.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I think project based learning with oral assessments of concepts </t>
+  </si>
+  <si>
+    <t>aviluhana@gmail.com</t>
+  </si>
+  <si>
+    <t>We can learn more practically.</t>
+  </si>
+  <si>
+    <t>I could add the projects in my CV and explain in interviews.</t>
+  </si>
+  <si>
+    <t>Gether information</t>
+  </si>
+  <si>
+    <t>Yes, because it is interesting for me to work on these.</t>
+  </si>
+  <si>
+    <t>Project-based assessments better reflect practical skills, creativity, effort, and teamwork than traditional tests, showing real-world learning more clearly.</t>
+  </si>
+  <si>
+    <t>I support the use of AI tools, especially in formats like projects or research tasks, where they enhance learning and creativity. Dishonesty depends more on intent than the tool itself. With proper guidance, AI can be a helpful part of the learning process.</t>
+  </si>
+  <si>
+    <t>My ideal assessment would combine projects, presentations, and reflective writing. This mix shows practical skills, creativity, communication, and how well I understand and apply what I've learned.</t>
+  </si>
+  <si>
+    <t>anadkatkanan1999@gmail.com</t>
+  </si>
+  <si>
+    <t>Performance-based assessment is better because it measures students’ ability to apply knowledge in real-world tasks, not just recall facts.</t>
+  </si>
+  <si>
+    <t>Completing a hands-on science project was a positive assessment experience because it allowed me to creatively apply what I had learned.</t>
+  </si>
+  <si>
+    <t>Traditional essay-based assessments can be frustrating because they often prioritize writing style over actual understanding or practical application of knowledge.</t>
+  </si>
+  <si>
+    <t>I found oral assessments stressful because of performance anxiety, but helpful for improving my communication and critical thinking skills.</t>
+  </si>
+  <si>
+    <t>Project-based assessments better showcase what I’ve learned by allowing me to apply knowledge in practical, real-world tasks.</t>
+  </si>
+  <si>
+    <t>Certain formats like multiple-choice exams can encourage dishonesty, while performance-based tasks discourage it by requiring original, hands-on work.</t>
+  </si>
+  <si>
+    <t>My ideal assessment would combine practical projects and reflective presentations to assess both applied skills and deep understanding.</t>
   </si>
 </sst>
 </file>
@@ -584,7 +785,7 @@
       <patternFill patternType="lightGray"/>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="12">
     <border/>
     <border>
       <left style="thin">
@@ -740,25 +941,11 @@
         <color rgb="FF442F65"/>
       </bottom>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFFFFFFF"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF442F65"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFFFFFFF"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF442F65"/>
-      </bottom>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="21">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -798,13 +985,28 @@
     <xf borderId="6" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
+    <xf borderId="7" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="8" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="9" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="6" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
     <xf borderId="10" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="11" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="12" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
   </cellXfs>
@@ -865,7 +1067,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:O16" displayName="Form_Responses" name="Form_Responses" id="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:O24" displayName="Form_Responses" name="Form_Responses" id="1">
   <tableColumns count="15">
     <tableColumn name="Timestamp" id="1"/>
     <tableColumn name="Email Address" id="2"/>
@@ -1792,50 +1994,408 @@
       <c r="O15" s="11"/>
     </row>
     <row r="16">
-      <c r="A16" s="13">
+      <c r="A16" s="5">
         <v>45875.484572719906</v>
       </c>
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="C16" s="14" t="s">
+      <c r="C16" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D16" s="14" t="s">
+      <c r="D16" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E16" s="14" t="s">
+      <c r="E16" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="F16" s="14" t="s">
+      <c r="F16" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="G16" s="14" t="s">
+      <c r="G16" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="H16" s="14" t="s">
+      <c r="H16" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="I16" s="14" t="s">
+      <c r="I16" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="J16" s="14" t="s">
+      <c r="J16" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="K16" s="14" t="s">
+      <c r="K16" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="L16" s="14" t="s">
+      <c r="L16" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="M16" s="14" t="s">
+      <c r="M16" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="N16" s="14" t="s">
+      <c r="N16" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="O16" s="15" t="s">
+      <c r="O16" s="7" t="s">
         <v>150</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="13">
+        <v>45875.510181875</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="F17" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="G17" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="H17" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="I17" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="J17" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="K17" s="14" t="s">
+        <v>157</v>
+      </c>
+      <c r="L17" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="M17" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="N17" s="14" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="15">
+        <v>45875.51506962963</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>159</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="F18" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="G18" s="16" t="s">
+        <v>161</v>
+      </c>
+      <c r="H18" s="16" t="s">
+        <v>162</v>
+      </c>
+      <c r="I18" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="J18" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="K18" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="L18" s="16" t="s">
+        <v>166</v>
+      </c>
+      <c r="M18" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="N18" s="16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="13">
+        <v>45875.57534203704</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="E19" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="F19" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="G19" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="H19" s="14" t="s">
+        <v>170</v>
+      </c>
+      <c r="I19" s="14" t="s">
+        <v>171</v>
+      </c>
+      <c r="J19" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="K19" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="L19" s="14" t="s">
+        <v>174</v>
+      </c>
+      <c r="M19" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="N19" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="O19" s="17" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="15">
+        <v>45875.58596581018</v>
+      </c>
+      <c r="B20" s="16" t="s">
+        <v>175</v>
+      </c>
+      <c r="C20" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="E20" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="F20" s="16" t="s">
+        <v>176</v>
+      </c>
+      <c r="G20" s="16" t="s">
+        <v>177</v>
+      </c>
+      <c r="H20" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="I20" s="16" t="s">
+        <v>179</v>
+      </c>
+      <c r="J20" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="K20" s="16" t="s">
+        <v>181</v>
+      </c>
+      <c r="L20" s="16" t="s">
+        <v>182</v>
+      </c>
+      <c r="M20" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="N20" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="O20" s="18" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="13">
+        <v>45875.59010585648</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>183</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E21" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="F21" s="14" t="s">
+        <v>184</v>
+      </c>
+      <c r="G21" s="14" t="s">
+        <v>185</v>
+      </c>
+      <c r="H21" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="I21" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="J21" s="14" t="s">
+        <v>187</v>
+      </c>
+      <c r="K21" s="14" t="s">
+        <v>188</v>
+      </c>
+      <c r="L21" s="14" t="s">
+        <v>189</v>
+      </c>
+      <c r="M21" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="N21" s="14" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="15">
+        <v>45875.60513386574</v>
+      </c>
+      <c r="B22" s="16" t="s">
+        <v>190</v>
+      </c>
+      <c r="C22" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="D22" s="16" t="s">
+        <v>191</v>
+      </c>
+      <c r="E22" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="F22" s="16" t="s">
+        <v>192</v>
+      </c>
+      <c r="G22" s="16" t="s">
+        <v>193</v>
+      </c>
+      <c r="H22" s="16" t="s">
+        <v>194</v>
+      </c>
+      <c r="I22" s="16" t="s">
+        <v>195</v>
+      </c>
+      <c r="J22" s="16" t="s">
+        <v>196</v>
+      </c>
+      <c r="K22" s="16" t="s">
+        <v>197</v>
+      </c>
+      <c r="L22" s="16" t="s">
+        <v>198</v>
+      </c>
+      <c r="M22" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="N22" s="16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="13">
+        <v>45875.616069814816</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>199</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="E23" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="F23" s="14" t="s">
+        <v>200</v>
+      </c>
+      <c r="G23" s="14" t="s">
+        <v>201</v>
+      </c>
+      <c r="H23" s="14" t="s">
+        <v>202</v>
+      </c>
+      <c r="I23" s="14" t="s">
+        <v>203</v>
+      </c>
+      <c r="J23" s="14" t="s">
+        <v>204</v>
+      </c>
+      <c r="K23" s="14" t="s">
+        <v>205</v>
+      </c>
+      <c r="L23" s="14" t="s">
+        <v>206</v>
+      </c>
+      <c r="M23" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="N23" s="14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="19">
+        <v>45875.78531871528</v>
+      </c>
+      <c r="B24" s="20" t="s">
+        <v>207</v>
+      </c>
+      <c r="C24" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D24" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="E24" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="F24" s="20" t="s">
+        <v>208</v>
+      </c>
+      <c r="G24" s="20" t="s">
+        <v>209</v>
+      </c>
+      <c r="H24" s="20" t="s">
+        <v>210</v>
+      </c>
+      <c r="I24" s="20" t="s">
+        <v>211</v>
+      </c>
+      <c r="J24" s="20" t="s">
+        <v>212</v>
+      </c>
+      <c r="K24" s="20" t="s">
+        <v>213</v>
+      </c>
+      <c r="L24" s="20" t="s">
+        <v>214</v>
+      </c>
+      <c r="M24" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="N24" s="20" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>